<commit_message>
RC detached added DH network with RC models
</commit_message>
<xml_diff>
--- a/Annex60.xlsx
+++ b/Annex60.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="10305" yWindow="45" windowWidth="10200" windowHeight="8115" activeTab="3"/>
+    <workbookView xWindow="10305" yWindow="45" windowWidth="10200" windowHeight="8115" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="S1_EPB2010" sheetId="2" r:id="rId1"/>
@@ -204,7 +204,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2253" uniqueCount="236">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2707" uniqueCount="238">
   <si>
     <t>W/m²K</t>
   </si>
@@ -1170,6 +1170,12 @@
   </si>
   <si>
     <t>Parameter reduced order SR2</t>
+  </si>
+  <si>
+    <t>Parameter reduced order D1</t>
+  </si>
+  <si>
+    <t>Parameter reduced order D2</t>
   </si>
 </sst>
 </file>
@@ -3945,8 +3951,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L52"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G36" sqref="G36"/>
+    <sheetView topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I23" sqref="I23:I24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5094,10 +5100,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O45"/>
+  <dimension ref="A1:X86"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="I43" sqref="I43"/>
+    <sheetView tabSelected="1" topLeftCell="I34" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="U2" sqref="U2:X86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5113,10 +5119,18 @@
     <col min="11" max="11" width="16.85546875" style="59" customWidth="1"/>
     <col min="12" max="12" width="3.42578125" style="59" customWidth="1"/>
     <col min="13" max="13" width="24.85546875" style="59" customWidth="1"/>
-    <col min="14" max="16384" width="9.140625" style="59"/>
+    <col min="14" max="16" width="9.140625" style="59"/>
+    <col min="17" max="17" width="21.5703125" style="59" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="2" style="59" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="51.85546875" style="59" customWidth="1"/>
+    <col min="20" max="20" width="9.140625" style="59" customWidth="1"/>
+    <col min="21" max="21" width="21.5703125" style="59" customWidth="1"/>
+    <col min="22" max="22" width="2" style="59" customWidth="1"/>
+    <col min="23" max="23" width="56.5703125" style="59" customWidth="1"/>
+    <col min="24" max="16384" width="9.140625" style="59"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
       <c r="I1" s="179" t="s">
         <v>129</v>
       </c>
@@ -5136,8 +5150,20 @@
       <c r="N1" s="168" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="2" spans="1:14" ht="18" x14ac:dyDescent="0.35">
+      <c r="Q1" s="240" t="s">
+        <v>236</v>
+      </c>
+      <c r="R1" s="240"/>
+      <c r="S1" s="240"/>
+      <c r="T1" s="240"/>
+      <c r="U1" s="240" t="s">
+        <v>237</v>
+      </c>
+      <c r="V1" s="240"/>
+      <c r="W1" s="240"/>
+      <c r="X1" s="240"/>
+    </row>
+    <row r="2" spans="1:24" ht="18" x14ac:dyDescent="0.35">
       <c r="A2" s="62"/>
       <c r="B2" s="62" t="s">
         <v>32</v>
@@ -5163,14 +5189,39 @@
         <v>118</v>
       </c>
       <c r="M2" s="83">
-        <f>C5</f>
-        <v>0</v>
+        <v>55.74</v>
       </c>
       <c r="N2" s="171" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="3" spans="1:14" ht="18" x14ac:dyDescent="0.35">
+      <c r="Q2" s="231" t="s">
+        <v>155</v>
+      </c>
+      <c r="R2" s="231" t="s">
+        <v>118</v>
+      </c>
+      <c r="S2" s="234">
+        <f>M27</f>
+        <v>1.8</v>
+      </c>
+      <c r="T2" s="230" t="s">
+        <v>119</v>
+      </c>
+      <c r="U2" s="231" t="s">
+        <v>155</v>
+      </c>
+      <c r="V2" s="231" t="s">
+        <v>118</v>
+      </c>
+      <c r="W2" s="234">
+        <f>S2</f>
+        <v>1.8</v>
+      </c>
+      <c r="X2" s="230" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="3" spans="1:24" ht="18" x14ac:dyDescent="0.35">
       <c r="A3" s="66" t="s">
         <v>35</v>
       </c>
@@ -5194,14 +5245,39 @@
         <v>118</v>
       </c>
       <c r="M3" s="172">
-        <f>D21</f>
-        <v>0</v>
+        <v>32.5</v>
       </c>
       <c r="N3" s="171" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="Q3" s="231" t="s">
+        <v>156</v>
+      </c>
+      <c r="R3" s="231" t="s">
+        <v>118</v>
+      </c>
+      <c r="S3" s="234">
+        <f>M28</f>
+        <v>4.8</v>
+      </c>
+      <c r="T3" s="230" t="s">
+        <v>119</v>
+      </c>
+      <c r="U3" s="231" t="s">
+        <v>156</v>
+      </c>
+      <c r="V3" s="231" t="s">
+        <v>118</v>
+      </c>
+      <c r="W3" s="234">
+        <f>S3</f>
+        <v>4.8</v>
+      </c>
+      <c r="X3" s="230" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A4" s="66" t="s">
         <v>37</v>
       </c>
@@ -5220,14 +5296,39 @@
         <v>118</v>
       </c>
       <c r="M4" s="172">
-        <f>D23</f>
-        <v>0</v>
+        <v>50.7</v>
       </c>
       <c r="N4" s="171" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="5" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Q4" s="231" t="s">
+        <v>157</v>
+      </c>
+      <c r="R4" s="231" t="s">
+        <v>118</v>
+      </c>
+      <c r="S4" s="234">
+        <f>M25</f>
+        <v>7.04</v>
+      </c>
+      <c r="T4" s="230" t="s">
+        <v>119</v>
+      </c>
+      <c r="U4" s="231" t="s">
+        <v>157</v>
+      </c>
+      <c r="V4" s="231" t="s">
+        <v>118</v>
+      </c>
+      <c r="W4" s="234">
+        <f>S4</f>
+        <v>7.04</v>
+      </c>
+      <c r="X4" s="230" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="5" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="74" t="s">
         <v>74</v>
       </c>
@@ -5247,14 +5348,39 @@
         <v>118</v>
       </c>
       <c r="M5" s="173">
-        <f>D10</f>
-        <v>0</v>
+        <v>6.29</v>
       </c>
       <c r="N5" s="171" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="6" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Q5" s="231" t="s">
+        <v>158</v>
+      </c>
+      <c r="R5" s="231" t="s">
+        <v>118</v>
+      </c>
+      <c r="S5" s="234">
+        <f>M26</f>
+        <v>5.64</v>
+      </c>
+      <c r="T5" s="230" t="s">
+        <v>119</v>
+      </c>
+      <c r="U5" s="231" t="s">
+        <v>158</v>
+      </c>
+      <c r="V5" s="231" t="s">
+        <v>118</v>
+      </c>
+      <c r="W5" s="234">
+        <f>S5</f>
+        <v>5.64</v>
+      </c>
+      <c r="X5" s="230" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="6" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="59" t="s">
         <v>38</v>
       </c>
@@ -5279,14 +5405,20 @@
         <v>118</v>
       </c>
       <c r="M6" s="173">
-        <f>D12</f>
-        <v>0</v>
+        <v>6.29</v>
       </c>
       <c r="N6" s="171" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="Q6"/>
+      <c r="R6" s="231"/>
+      <c r="T6" s="230"/>
+      <c r="U6"/>
+      <c r="V6" s="231"/>
+      <c r="W6" s="234"/>
+      <c r="X6" s="230"/>
+    </row>
+    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
       <c r="I7" s="181" t="s">
         <v>129</v>
       </c>
@@ -5300,14 +5432,39 @@
         <v>118</v>
       </c>
       <c r="M7" s="173">
-        <f>C4</f>
-        <v>0</v>
+        <v>236.4</v>
       </c>
       <c r="N7" s="171" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="Q7" s="231" t="s">
+        <v>159</v>
+      </c>
+      <c r="R7" s="231" t="s">
+        <v>118</v>
+      </c>
+      <c r="S7" s="234">
+        <f>M14</f>
+        <v>0.8</v>
+      </c>
+      <c r="T7" s="230" t="s">
+        <v>119</v>
+      </c>
+      <c r="U7" s="231" t="s">
+        <v>159</v>
+      </c>
+      <c r="V7" s="231" t="s">
+        <v>118</v>
+      </c>
+      <c r="W7" s="234">
+        <f>S7</f>
+        <v>0.8</v>
+      </c>
+      <c r="X7" s="230" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
       <c r="B8" s="79" t="s">
         <v>35</v>
       </c>
@@ -5333,14 +5490,39 @@
         <v>118</v>
       </c>
       <c r="M8" s="173">
-        <f t="shared" ref="M8:M15" si="0">C9</f>
-        <v>0</v>
+        <v>31.8</v>
       </c>
       <c r="N8" s="171" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="Q8" s="231" t="s">
+        <v>160</v>
+      </c>
+      <c r="R8" s="231" t="s">
+        <v>118</v>
+      </c>
+      <c r="S8" s="104">
+        <f>M15</f>
+        <v>2.9</v>
+      </c>
+      <c r="T8" s="230" t="s">
+        <v>119</v>
+      </c>
+      <c r="U8" s="231" t="s">
+        <v>160</v>
+      </c>
+      <c r="V8" s="231" t="s">
+        <v>118</v>
+      </c>
+      <c r="W8" s="234">
+        <f>S8</f>
+        <v>2.9</v>
+      </c>
+      <c r="X8" s="230" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A9" s="80" t="s">
         <v>39</v>
       </c>
@@ -5350,7 +5532,7 @@
         <v>59</v>
       </c>
       <c r="E9" s="83">
-        <f t="shared" ref="E9:E24" si="1">SUM(B9:D9)</f>
+        <f t="shared" ref="E9:E24" si="0">SUM(B9:D9)</f>
         <v>0</v>
       </c>
       <c r="G9" s="65">
@@ -5369,14 +5551,39 @@
         <v>118</v>
       </c>
       <c r="M9" s="173">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <v>18.2</v>
       </c>
       <c r="N9" s="171" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="Q9" s="231" t="s">
+        <v>161</v>
+      </c>
+      <c r="R9" s="231" t="s">
+        <v>118</v>
+      </c>
+      <c r="S9" s="234">
+        <f>M12</f>
+        <v>4.3</v>
+      </c>
+      <c r="T9" s="230" t="s">
+        <v>119</v>
+      </c>
+      <c r="U9" s="231" t="s">
+        <v>161</v>
+      </c>
+      <c r="V9" s="231" t="s">
+        <v>118</v>
+      </c>
+      <c r="W9" s="234">
+        <f>S9</f>
+        <v>4.3</v>
+      </c>
+      <c r="X9" s="230" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A10" s="80" t="s">
         <v>40</v>
       </c>
@@ -5384,7 +5591,7 @@
       <c r="C10" s="83"/>
       <c r="D10" s="85"/>
       <c r="E10" s="83">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="G10" s="65">
@@ -5403,14 +5610,39 @@
         <v>118</v>
       </c>
       <c r="M10" s="173">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <v>36.1</v>
       </c>
       <c r="N10" s="171" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="Q10" s="231" t="s">
+        <v>162</v>
+      </c>
+      <c r="R10" s="231" t="s">
+        <v>118</v>
+      </c>
+      <c r="S10" s="234">
+        <f>M13</f>
+        <v>2.7</v>
+      </c>
+      <c r="T10" s="230" t="s">
+        <v>119</v>
+      </c>
+      <c r="U10" s="231" t="s">
+        <v>162</v>
+      </c>
+      <c r="V10" s="231" t="s">
+        <v>118</v>
+      </c>
+      <c r="W10" s="234">
+        <f>S10</f>
+        <v>2.7</v>
+      </c>
+      <c r="X10" s="230" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A11" s="80" t="s">
         <v>41</v>
       </c>
@@ -5439,14 +5671,19 @@
         <v>118</v>
       </c>
       <c r="M11" s="173">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="N11" s="171" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="Q11"/>
+      <c r="R11" s="231"/>
+      <c r="T11" s="230"/>
+      <c r="U11"/>
+      <c r="V11" s="231"/>
+      <c r="X11" s="230"/>
+    </row>
+    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A12" s="88" t="s">
         <v>42</v>
       </c>
@@ -5454,7 +5691,7 @@
       <c r="C12" s="90"/>
       <c r="D12" s="87"/>
       <c r="E12" s="90">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="G12" s="65">
@@ -5473,14 +5710,23 @@
         <v>118</v>
       </c>
       <c r="M12" s="173">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4.3</v>
       </c>
       <c r="N12" s="171" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="Q12" s="232" t="s">
+        <v>154</v>
+      </c>
+      <c r="R12" s="231"/>
+      <c r="T12" s="230"/>
+      <c r="U12" s="232" t="s">
+        <v>154</v>
+      </c>
+      <c r="V12" s="231"/>
+      <c r="X12" s="230"/>
+    </row>
+    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A13" s="91" t="s">
         <v>43</v>
       </c>
@@ -5490,7 +5736,7 @@
         <v>59</v>
       </c>
       <c r="E13" s="92">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="I13" s="181" t="s">
@@ -5506,14 +5752,39 @@
         <v>118</v>
       </c>
       <c r="M13" s="173">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2.7</v>
       </c>
       <c r="N13" s="171" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="Q13" s="178" t="s">
+        <v>194</v>
+      </c>
+      <c r="R13" s="230" t="s">
+        <v>118</v>
+      </c>
+      <c r="S13" s="59">
+        <f>S3*S1_EPB2010!$C$55*0.25*0.8</f>
+        <v>0.7248</v>
+      </c>
+      <c r="T13" s="230" t="s">
+        <v>119</v>
+      </c>
+      <c r="U13" s="178" t="s">
+        <v>194</v>
+      </c>
+      <c r="V13" s="230" t="s">
+        <v>118</v>
+      </c>
+      <c r="W13" s="59">
+        <f>W3*'S2_1946-1970'!$C$51*0.25*0.8</f>
+        <v>0.7248</v>
+      </c>
+      <c r="X13" s="230" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A14" s="80" t="s">
         <v>44</v>
       </c>
@@ -5523,7 +5794,7 @@
         <v>59</v>
       </c>
       <c r="E14" s="69">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="I14" s="181" t="s">
@@ -5539,14 +5810,39 @@
         <v>118</v>
       </c>
       <c r="M14" s="173">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.8</v>
       </c>
       <c r="N14" s="171" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="Q14" s="178" t="s">
+        <v>195</v>
+      </c>
+      <c r="R14" s="230" t="s">
+        <v>118</v>
+      </c>
+      <c r="S14" s="59">
+        <f>S2*S1_EPB2010!$C$55*0.25*0.8</f>
+        <v>0.27179999999999999</v>
+      </c>
+      <c r="T14" s="230" t="s">
+        <v>119</v>
+      </c>
+      <c r="U14" s="178" t="s">
+        <v>195</v>
+      </c>
+      <c r="V14" s="230" t="s">
+        <v>118</v>
+      </c>
+      <c r="W14" s="59">
+        <f>W2*'S2_1946-1970'!$C$51*0.25*0.8</f>
+        <v>0.27179999999999999</v>
+      </c>
+      <c r="X14" s="230" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="15" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A15" s="80" t="s">
         <v>45</v>
       </c>
@@ -5556,7 +5852,7 @@
         <v>59</v>
       </c>
       <c r="E15" s="69">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="I15" s="181" t="s">
@@ -5572,14 +5868,39 @@
         <v>118</v>
       </c>
       <c r="M15" s="173">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2.9</v>
       </c>
       <c r="N15" s="171" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="Q15" s="178" t="s">
+        <v>196</v>
+      </c>
+      <c r="R15" s="230" t="s">
+        <v>118</v>
+      </c>
+      <c r="S15" s="59">
+        <f>S4*S1_EPB2010!$C$55*0.25*0.8</f>
+        <v>1.06304</v>
+      </c>
+      <c r="T15" s="230" t="s">
+        <v>119</v>
+      </c>
+      <c r="U15" s="178" t="s">
+        <v>196</v>
+      </c>
+      <c r="V15" s="230" t="s">
+        <v>118</v>
+      </c>
+      <c r="W15" s="59">
+        <f>W4*'S2_1946-1970'!$C$51*0.25*0.8</f>
+        <v>1.06304</v>
+      </c>
+      <c r="X15" s="230" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A16" s="88" t="s">
         <v>46</v>
       </c>
@@ -5589,7 +5910,7 @@
         <v>59</v>
       </c>
       <c r="E16" s="96">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="I16" s="181" t="s">
@@ -5605,14 +5926,39 @@
         <v>118</v>
       </c>
       <c r="M16" s="172">
-        <f>C21</f>
-        <v>0</v>
+        <v>13.2</v>
       </c>
       <c r="N16" s="171" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q16" s="178" t="s">
+        <v>197</v>
+      </c>
+      <c r="R16" s="230" t="s">
+        <v>118</v>
+      </c>
+      <c r="S16" s="59">
+        <f>S5*S1_EPB2010!$C$55*0.25*0.8</f>
+        <v>0.85163999999999995</v>
+      </c>
+      <c r="T16" s="230" t="s">
+        <v>119</v>
+      </c>
+      <c r="U16" s="178" t="s">
+        <v>197</v>
+      </c>
+      <c r="V16" s="230" t="s">
+        <v>118</v>
+      </c>
+      <c r="W16" s="59">
+        <f>W5*'S2_1946-1970'!$C$51*0.25*0.8</f>
+        <v>0.85163999999999995</v>
+      </c>
+      <c r="X16" s="230" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="17" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A17" s="91" t="s">
         <v>47</v>
       </c>
@@ -5626,7 +5972,7 @@
         <v>59</v>
       </c>
       <c r="E17" s="92">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="I17" s="181" t="s">
@@ -5642,14 +5988,39 @@
         <v>118</v>
       </c>
       <c r="M17" s="172">
-        <f>C23</f>
-        <v>0</v>
+        <v>13.2</v>
       </c>
       <c r="N17" s="171" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q17" s="178" t="s">
+        <v>198</v>
+      </c>
+      <c r="R17" s="230" t="s">
+        <v>118</v>
+      </c>
+      <c r="S17" s="59">
+        <f>S13</f>
+        <v>0.7248</v>
+      </c>
+      <c r="T17" s="230" t="s">
+        <v>119</v>
+      </c>
+      <c r="U17" s="178" t="s">
+        <v>198</v>
+      </c>
+      <c r="V17" s="230" t="s">
+        <v>118</v>
+      </c>
+      <c r="W17" s="59">
+        <f>W13</f>
+        <v>0.7248</v>
+      </c>
+      <c r="X17" s="230" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="18" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A18" s="80" t="s">
         <v>48</v>
       </c>
@@ -5664,7 +6035,7 @@
         <v>59</v>
       </c>
       <c r="E18" s="69">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>1.8</v>
       </c>
       <c r="I18" s="181" t="s">
@@ -5680,14 +6051,39 @@
         <v>118</v>
       </c>
       <c r="M18" s="172">
-        <f>C28</f>
-        <v>0</v>
+        <v>56.5</v>
       </c>
       <c r="N18" s="171" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q18" s="178" t="s">
+        <v>199</v>
+      </c>
+      <c r="R18" s="230" t="s">
+        <v>118</v>
+      </c>
+      <c r="S18" s="59">
+        <f t="shared" ref="S18:S20" si="1">S14</f>
+        <v>0.27179999999999999</v>
+      </c>
+      <c r="T18" s="230" t="s">
+        <v>119</v>
+      </c>
+      <c r="U18" s="178" t="s">
+        <v>199</v>
+      </c>
+      <c r="V18" s="230" t="s">
+        <v>118</v>
+      </c>
+      <c r="W18" s="59">
+        <f t="shared" ref="W18:W20" si="2">W14</f>
+        <v>0.27179999999999999</v>
+      </c>
+      <c r="X18" s="230" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="19" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A19" s="80" t="s">
         <v>49</v>
       </c>
@@ -5702,7 +6098,7 @@
         <v>59</v>
       </c>
       <c r="E19" s="69">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>1.8</v>
       </c>
       <c r="I19" s="181" t="s">
@@ -5718,14 +6114,39 @@
         <v>118</v>
       </c>
       <c r="M19" s="172">
-        <f>D27</f>
-        <v>0</v>
+        <v>71.3</v>
       </c>
       <c r="N19" s="171" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q19" s="178" t="s">
+        <v>200</v>
+      </c>
+      <c r="R19" s="230" t="s">
+        <v>118</v>
+      </c>
+      <c r="S19" s="59">
+        <f t="shared" si="1"/>
+        <v>1.06304</v>
+      </c>
+      <c r="T19" s="230" t="s">
+        <v>119</v>
+      </c>
+      <c r="U19" s="178" t="s">
+        <v>200</v>
+      </c>
+      <c r="V19" s="230" t="s">
+        <v>118</v>
+      </c>
+      <c r="W19" s="59">
+        <f t="shared" si="2"/>
+        <v>1.06304</v>
+      </c>
+      <c r="X19" s="230" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="20" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A20" s="88" t="s">
         <v>50</v>
       </c>
@@ -5739,7 +6160,7 @@
         <v>59</v>
       </c>
       <c r="E20" s="96">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="I20" s="181" t="s">
@@ -5755,14 +6176,39 @@
         <v>118</v>
       </c>
       <c r="M20" s="173">
-        <f>C3</f>
-        <v>0</v>
+        <v>236.4</v>
       </c>
       <c r="N20" s="171" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q20" s="178" t="s">
+        <v>201</v>
+      </c>
+      <c r="R20" s="230" t="s">
+        <v>118</v>
+      </c>
+      <c r="S20" s="59">
+        <f t="shared" si="1"/>
+        <v>0.85163999999999995</v>
+      </c>
+      <c r="T20" s="230" t="s">
+        <v>119</v>
+      </c>
+      <c r="U20" s="178" t="s">
+        <v>201</v>
+      </c>
+      <c r="V20" s="230" t="s">
+        <v>118</v>
+      </c>
+      <c r="W20" s="59">
+        <f t="shared" si="2"/>
+        <v>0.85163999999999995</v>
+      </c>
+      <c r="X20" s="230" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="21" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A21" s="91" t="s">
         <v>51</v>
       </c>
@@ -5792,14 +6238,37 @@
         <v>118</v>
       </c>
       <c r="M21" s="172">
-        <f t="shared" ref="M21:M28" si="2">B9</f>
-        <v>0</v>
+        <v>24.76</v>
       </c>
       <c r="N21" s="171" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q21" s="178" t="s">
+        <v>202</v>
+      </c>
+      <c r="R21" s="230" t="s">
+        <v>118</v>
+      </c>
+      <c r="S21" s="59">
+        <v>0</v>
+      </c>
+      <c r="T21" s="230" t="s">
+        <v>119</v>
+      </c>
+      <c r="U21" s="178" t="s">
+        <v>202</v>
+      </c>
+      <c r="V21" s="230" t="s">
+        <v>118</v>
+      </c>
+      <c r="W21" s="59">
+        <v>0</v>
+      </c>
+      <c r="X21" s="230" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="22" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A22" s="80" t="s">
         <v>53</v>
       </c>
@@ -5813,7 +6282,7 @@
         <v>59</v>
       </c>
       <c r="E22" s="86">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F22" s="64"/>
@@ -5831,14 +6300,37 @@
         <v>118</v>
       </c>
       <c r="M22" s="172">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <v>15.26</v>
       </c>
       <c r="N22" s="171" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q22" s="178" t="s">
+        <v>203</v>
+      </c>
+      <c r="R22" s="230" t="s">
+        <v>118</v>
+      </c>
+      <c r="S22" s="59">
+        <v>0</v>
+      </c>
+      <c r="T22" s="230" t="s">
+        <v>119</v>
+      </c>
+      <c r="U22" s="178" t="s">
+        <v>203</v>
+      </c>
+      <c r="V22" s="230" t="s">
+        <v>118</v>
+      </c>
+      <c r="W22" s="59">
+        <v>0</v>
+      </c>
+      <c r="X22" s="230" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="23" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A23" s="80" t="s">
         <v>54</v>
       </c>
@@ -5848,7 +6340,7 @@
       <c r="C23" s="83"/>
       <c r="D23" s="85"/>
       <c r="E23" s="83">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F23" s="64" t="s">
@@ -5868,14 +6360,37 @@
         <v>118</v>
       </c>
       <c r="M23" s="172">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="N23" s="171" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q23" s="178" t="s">
+        <v>204</v>
+      </c>
+      <c r="R23" s="230" t="s">
+        <v>118</v>
+      </c>
+      <c r="S23" s="59">
+        <v>0</v>
+      </c>
+      <c r="T23" s="230" t="s">
+        <v>119</v>
+      </c>
+      <c r="U23" s="178" t="s">
+        <v>204</v>
+      </c>
+      <c r="V23" s="230" t="s">
+        <v>118</v>
+      </c>
+      <c r="W23" s="59">
+        <v>0</v>
+      </c>
+      <c r="X23" s="230" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="24" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A24" s="88" t="s">
         <v>55</v>
       </c>
@@ -5889,7 +6404,7 @@
         <v>59</v>
       </c>
       <c r="E24" s="96">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="I24" s="181" t="s">
@@ -5905,14 +6420,37 @@
         <v>118</v>
       </c>
       <c r="M24" s="172">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <v>16.100000000000001</v>
       </c>
       <c r="N24" s="171" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q24" s="178" t="s">
+        <v>205</v>
+      </c>
+      <c r="R24" s="230" t="s">
+        <v>118</v>
+      </c>
+      <c r="S24" s="59">
+        <v>0</v>
+      </c>
+      <c r="T24" s="230" t="s">
+        <v>119</v>
+      </c>
+      <c r="U24" s="178" t="s">
+        <v>205</v>
+      </c>
+      <c r="V24" s="230" t="s">
+        <v>118</v>
+      </c>
+      <c r="W24" s="59">
+        <v>0</v>
+      </c>
+      <c r="X24" s="230" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="25" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A25" s="103" t="s">
         <v>56</v>
       </c>
@@ -5940,14 +6478,39 @@
         <v>118</v>
       </c>
       <c r="M25" s="172">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <v>7.04</v>
       </c>
       <c r="N25" s="171" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q25" s="178" t="s">
+        <v>206</v>
+      </c>
+      <c r="R25" s="230" t="s">
+        <v>118</v>
+      </c>
+      <c r="S25" s="59">
+        <f>S13</f>
+        <v>0.7248</v>
+      </c>
+      <c r="T25" s="230" t="s">
+        <v>119</v>
+      </c>
+      <c r="U25" s="178" t="s">
+        <v>206</v>
+      </c>
+      <c r="V25" s="230" t="s">
+        <v>118</v>
+      </c>
+      <c r="W25" s="59">
+        <f>W13</f>
+        <v>0.7248</v>
+      </c>
+      <c r="X25" s="230" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="26" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A26" s="105" t="s">
         <v>57</v>
       </c>
@@ -5971,14 +6534,39 @@
         <v>118</v>
       </c>
       <c r="M26" s="172">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <v>5.64</v>
       </c>
       <c r="N26" s="171" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q26" s="178" t="s">
+        <v>207</v>
+      </c>
+      <c r="R26" s="230" t="s">
+        <v>118</v>
+      </c>
+      <c r="S26" s="59">
+        <f t="shared" ref="S26:S32" si="3">S14</f>
+        <v>0.27179999999999999</v>
+      </c>
+      <c r="T26" s="230" t="s">
+        <v>119</v>
+      </c>
+      <c r="U26" s="178" t="s">
+        <v>207</v>
+      </c>
+      <c r="V26" s="230" t="s">
+        <v>118</v>
+      </c>
+      <c r="W26" s="59">
+        <f t="shared" ref="W26:W32" si="4">W14</f>
+        <v>0.27179999999999999</v>
+      </c>
+      <c r="X26" s="230" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="27" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A27" s="79" t="s">
         <v>58</v>
       </c>
@@ -6000,14 +6588,39 @@
         <v>118</v>
       </c>
       <c r="M27" s="172">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1.8</v>
       </c>
       <c r="N27" s="171" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q27" s="178" t="s">
+        <v>208</v>
+      </c>
+      <c r="R27" s="230" t="s">
+        <v>118</v>
+      </c>
+      <c r="S27" s="59">
+        <f t="shared" si="3"/>
+        <v>1.06304</v>
+      </c>
+      <c r="T27" s="230" t="s">
+        <v>119</v>
+      </c>
+      <c r="U27" s="178" t="s">
+        <v>208</v>
+      </c>
+      <c r="V27" s="230" t="s">
+        <v>118</v>
+      </c>
+      <c r="W27" s="59">
+        <f t="shared" si="4"/>
+        <v>1.06304</v>
+      </c>
+      <c r="X27" s="230" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="28" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A28" s="79" t="s">
         <v>60</v>
       </c>
@@ -6028,14 +6641,39 @@
         <v>118</v>
       </c>
       <c r="M28" s="172">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <v>4.8</v>
       </c>
       <c r="N28" s="171" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q28" s="178" t="s">
+        <v>209</v>
+      </c>
+      <c r="R28" s="230" t="s">
+        <v>118</v>
+      </c>
+      <c r="S28" s="59">
+        <f t="shared" si="3"/>
+        <v>0.85163999999999995</v>
+      </c>
+      <c r="T28" s="230" t="s">
+        <v>119</v>
+      </c>
+      <c r="U28" s="178" t="s">
+        <v>209</v>
+      </c>
+      <c r="V28" s="230" t="s">
+        <v>118</v>
+      </c>
+      <c r="W28" s="59">
+        <f t="shared" si="4"/>
+        <v>0.85163999999999995</v>
+      </c>
+      <c r="X28" s="230" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="29" spans="1:24" x14ac:dyDescent="0.25">
       <c r="E29" s="98"/>
       <c r="I29" s="181" t="s">
         <v>129</v>
@@ -6050,7 +6688,6 @@
         <v>118</v>
       </c>
       <c r="M29" s="172">
-        <f>B19</f>
         <v>1.8</v>
       </c>
       <c r="N29" s="171" t="s">
@@ -6059,8 +6696,34 @@
       <c r="O29" s="212" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q29" s="178" t="s">
+        <v>210</v>
+      </c>
+      <c r="R29" s="230" t="s">
+        <v>118</v>
+      </c>
+      <c r="S29" s="59">
+        <f t="shared" si="3"/>
+        <v>0.7248</v>
+      </c>
+      <c r="T29" s="230" t="s">
+        <v>119</v>
+      </c>
+      <c r="U29" s="178" t="s">
+        <v>210</v>
+      </c>
+      <c r="V29" s="230" t="s">
+        <v>118</v>
+      </c>
+      <c r="W29" s="59">
+        <f t="shared" si="4"/>
+        <v>0.7248</v>
+      </c>
+      <c r="X29" s="230" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="30" spans="1:24" x14ac:dyDescent="0.25">
       <c r="I30" s="181" t="s">
         <v>129</v>
       </c>
@@ -6074,14 +6737,39 @@
         <v>118</v>
       </c>
       <c r="M30" s="172">
-        <f>B25</f>
-        <v>0</v>
+        <v>71.3</v>
       </c>
       <c r="N30" s="171" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="31" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Q30" s="178" t="s">
+        <v>211</v>
+      </c>
+      <c r="R30" s="230" t="s">
+        <v>118</v>
+      </c>
+      <c r="S30" s="59">
+        <f t="shared" si="3"/>
+        <v>0.27179999999999999</v>
+      </c>
+      <c r="T30" s="230" t="s">
+        <v>119</v>
+      </c>
+      <c r="U30" s="178" t="s">
+        <v>211</v>
+      </c>
+      <c r="V30" s="230" t="s">
+        <v>118</v>
+      </c>
+      <c r="W30" s="59">
+        <f t="shared" si="4"/>
+        <v>0.27179999999999999</v>
+      </c>
+      <c r="X30" s="230" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="31" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C31" s="109" t="s">
         <v>75</v>
       </c>
@@ -6101,14 +6789,39 @@
         <v>118</v>
       </c>
       <c r="M31" s="172">
-        <f>B26</f>
-        <v>0</v>
+        <v>40.5</v>
       </c>
       <c r="N31" s="171" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q31" s="178" t="s">
+        <v>212</v>
+      </c>
+      <c r="R31" s="230" t="s">
+        <v>118</v>
+      </c>
+      <c r="S31" s="59">
+        <f t="shared" si="3"/>
+        <v>1.06304</v>
+      </c>
+      <c r="T31" s="230" t="s">
+        <v>119</v>
+      </c>
+      <c r="U31" s="178" t="s">
+        <v>212</v>
+      </c>
+      <c r="V31" s="230" t="s">
+        <v>118</v>
+      </c>
+      <c r="W31" s="59">
+        <f t="shared" si="4"/>
+        <v>1.06304</v>
+      </c>
+      <c r="X31" s="230" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="32" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A32" s="111" t="s">
         <v>62</v>
       </c>
@@ -6134,14 +6847,39 @@
         <v>118</v>
       </c>
       <c r="M32" s="172">
-        <f>B28</f>
-        <v>0</v>
+        <v>58.65</v>
       </c>
       <c r="N32" s="171" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="33" spans="1:14" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Q32" s="178" t="s">
+        <v>213</v>
+      </c>
+      <c r="R32" s="230" t="s">
+        <v>118</v>
+      </c>
+      <c r="S32" s="59">
+        <f t="shared" si="3"/>
+        <v>0.85163999999999995</v>
+      </c>
+      <c r="T32" s="230" t="s">
+        <v>119</v>
+      </c>
+      <c r="U32" s="178" t="s">
+        <v>213</v>
+      </c>
+      <c r="V32" s="230" t="s">
+        <v>118</v>
+      </c>
+      <c r="W32" s="59">
+        <f t="shared" si="4"/>
+        <v>0.85163999999999995</v>
+      </c>
+      <c r="X32" s="230" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="33" spans="1:24" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="114" t="s">
         <v>63</v>
       </c>
@@ -6167,14 +6905,19 @@
         <v>118</v>
       </c>
       <c r="M33" s="177">
-        <f>B27</f>
-        <v>0</v>
+        <v>71.3</v>
       </c>
       <c r="N33" s="176" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="Q33"/>
+      <c r="R33" s="231"/>
+      <c r="T33" s="230"/>
+      <c r="U33"/>
+      <c r="V33" s="231"/>
+      <c r="X33" s="230"/>
+    </row>
+    <row r="34" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A34" s="114" t="s">
         <v>64</v>
       </c>
@@ -6187,8 +6930,34 @@
         <f>ABS((C34-B34)/C34*100)</f>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="Q34" s="233" t="s">
+        <v>163</v>
+      </c>
+      <c r="R34" s="231" t="s">
+        <v>118</v>
+      </c>
+      <c r="S34" s="236">
+        <f>$M$17*1.204*1012*5</f>
+        <v>80417.567999999999</v>
+      </c>
+      <c r="T34" s="230" t="s">
+        <v>119</v>
+      </c>
+      <c r="U34" s="233" t="s">
+        <v>163</v>
+      </c>
+      <c r="V34" s="231" t="s">
+        <v>118</v>
+      </c>
+      <c r="W34" s="236">
+        <f>$M$17*1.204*1012*5</f>
+        <v>80417.567999999999</v>
+      </c>
+      <c r="X34" s="230" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="35" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A35" s="114" t="s">
         <v>65</v>
       </c>
@@ -6201,8 +6970,34 @@
         <f>ABS((C35-B35)/C35*100)</f>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="36" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Q35" s="233" t="s">
+        <v>164</v>
+      </c>
+      <c r="R35" s="231" t="s">
+        <v>118</v>
+      </c>
+      <c r="S35" s="236">
+        <f>SUM($M$21:$M$24)*SUM(S1_EPB2010!$I$7:$I$8)</f>
+        <v>10019200.800000003</v>
+      </c>
+      <c r="T35" s="230" t="s">
+        <v>119</v>
+      </c>
+      <c r="U35" s="233" t="s">
+        <v>164</v>
+      </c>
+      <c r="V35" s="231" t="s">
+        <v>118</v>
+      </c>
+      <c r="W35" s="236">
+        <f>SUM($M$21:$M24)*SUM('S2_1946-1970'!$I$6:$I$7)</f>
+        <v>20146912.800000001</v>
+      </c>
+      <c r="X35" s="230" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="36" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="121" t="s">
         <v>67</v>
       </c>
@@ -6223,8 +7018,34 @@
       <c r="L36" s="239"/>
       <c r="M36" s="239"/>
       <c r="N36" s="239"/>
-    </row>
-    <row r="37" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Q36" s="233" t="s">
+        <v>165</v>
+      </c>
+      <c r="R36" s="231" t="s">
+        <v>118</v>
+      </c>
+      <c r="S36" s="236">
+        <f>SUM($M$32)*SUM(S1_EPB2010!$I$33:$I$35)</f>
+        <v>11035584</v>
+      </c>
+      <c r="T36" s="230" t="s">
+        <v>119</v>
+      </c>
+      <c r="U36" s="233" t="s">
+        <v>165</v>
+      </c>
+      <c r="V36" s="231" t="s">
+        <v>118</v>
+      </c>
+      <c r="W36" s="236">
+        <f>SUM($M$32)*SUM('S2_1946-1970'!$I$29:$I$31)</f>
+        <v>14681268</v>
+      </c>
+      <c r="X36" s="230" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="37" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C37" s="93"/>
       <c r="D37" s="116"/>
       <c r="I37" s="239"/>
@@ -6233,8 +7054,34 @@
       <c r="L37" s="239"/>
       <c r="M37" s="239"/>
       <c r="N37" s="239"/>
-    </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="Q37" s="233" t="s">
+        <v>166</v>
+      </c>
+      <c r="R37" s="231" t="s">
+        <v>118</v>
+      </c>
+      <c r="S37" s="235">
+        <f>SUM($M$30)*SUM(S1_EPB2010!$I$26:$I$27)</f>
+        <v>6562452</v>
+      </c>
+      <c r="T37" s="230" t="s">
+        <v>119</v>
+      </c>
+      <c r="U37" s="233" t="s">
+        <v>166</v>
+      </c>
+      <c r="V37" s="231" t="s">
+        <v>118</v>
+      </c>
+      <c r="W37" s="235">
+        <f>SUM($M$30)*SUM('S2_1946-1970'!$I$37:$I$38)</f>
+        <v>29916054</v>
+      </c>
+      <c r="X37" s="230" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="38" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A38" s="111" t="s">
         <v>32</v>
       </c>
@@ -6253,8 +7100,14 @@
       <c r="L38" s="239"/>
       <c r="M38" s="239"/>
       <c r="N38" s="239"/>
-    </row>
-    <row r="39" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Q38"/>
+      <c r="R38" s="231"/>
+      <c r="T38" s="230"/>
+      <c r="U38"/>
+      <c r="V38" s="231"/>
+      <c r="X38" s="230"/>
+    </row>
+    <row r="39" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="121" t="s">
         <v>33</v>
       </c>
@@ -6273,39 +7126,1247 @@
       <c r="K39" s="213"/>
       <c r="L39" s="213"/>
       <c r="M39" s="213"/>
-    </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="Q39" s="233" t="s">
+        <v>167</v>
+      </c>
+      <c r="R39" s="231" t="s">
+        <v>118</v>
+      </c>
+      <c r="S39" s="237">
+        <v>0.05</v>
+      </c>
+      <c r="T39" s="230" t="s">
+        <v>119</v>
+      </c>
+      <c r="U39" s="233" t="s">
+        <v>167</v>
+      </c>
+      <c r="V39" s="231" t="s">
+        <v>118</v>
+      </c>
+      <c r="W39" s="237">
+        <v>0.05</v>
+      </c>
+      <c r="X39" s="230" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="40" spans="1:24" x14ac:dyDescent="0.25">
       <c r="C40" s="59" t="s">
         <v>68</v>
       </c>
       <c r="D40" s="124" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="Q40" s="233" t="s">
+        <v>168</v>
+      </c>
+      <c r="R40" s="231" t="s">
+        <v>118</v>
+      </c>
+      <c r="S40" s="237">
+        <v>0.1</v>
+      </c>
+      <c r="T40" s="230" t="s">
+        <v>119</v>
+      </c>
+      <c r="U40" s="233" t="s">
+        <v>168</v>
+      </c>
+      <c r="V40" s="231" t="s">
+        <v>118</v>
+      </c>
+      <c r="W40" s="237">
+        <v>0.1</v>
+      </c>
+      <c r="X40" s="230" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="41" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Q41" s="233" t="s">
+        <v>169</v>
+      </c>
+      <c r="R41" s="231" t="s">
+        <v>118</v>
+      </c>
+      <c r="S41" s="237">
+        <v>0.7</v>
+      </c>
+      <c r="T41" s="230" t="s">
+        <v>119</v>
+      </c>
+      <c r="U41" s="233" t="s">
+        <v>169</v>
+      </c>
+      <c r="V41" s="231" t="s">
+        <v>118</v>
+      </c>
+      <c r="W41" s="237">
+        <v>0.7</v>
+      </c>
+      <c r="X41" s="230" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="42" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A42" s="125"/>
       <c r="B42" s="104"/>
       <c r="D42" s="104"/>
       <c r="E42" s="126"/>
-    </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="Q42" s="233" t="s">
+        <v>170</v>
+      </c>
+      <c r="R42" s="231" t="s">
+        <v>118</v>
+      </c>
+      <c r="S42" s="237">
+        <v>0.05</v>
+      </c>
+      <c r="T42" s="230" t="s">
+        <v>119</v>
+      </c>
+      <c r="U42" s="233" t="s">
+        <v>170</v>
+      </c>
+      <c r="V42" s="231" t="s">
+        <v>118</v>
+      </c>
+      <c r="W42" s="237">
+        <v>0.05</v>
+      </c>
+      <c r="X42" s="230" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="43" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A43" s="127"/>
       <c r="B43" s="104"/>
       <c r="E43" s="104"/>
       <c r="G43" s="104"/>
-    </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="Q43"/>
+      <c r="R43" s="231"/>
+      <c r="T43" s="230"/>
+      <c r="U43"/>
+      <c r="V43" s="231"/>
+      <c r="X43" s="230"/>
+    </row>
+    <row r="44" spans="1:24" x14ac:dyDescent="0.25">
       <c r="B44" s="104"/>
       <c r="E44" s="104"/>
       <c r="G44" s="104"/>
-    </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="Q44" s="233" t="s">
+        <v>171</v>
+      </c>
+      <c r="R44" s="231" t="s">
+        <v>118</v>
+      </c>
+      <c r="S44" s="59">
+        <f>SUM($M$21:$M$24)*(1/(1/6+SUM(S1_EPB2010!$H$7:$H$8)))</f>
+        <v>159.05045045045043</v>
+      </c>
+      <c r="T44" s="230" t="s">
+        <v>119</v>
+      </c>
+      <c r="U44" s="233" t="s">
+        <v>171</v>
+      </c>
+      <c r="V44" s="231" t="s">
+        <v>118</v>
+      </c>
+      <c r="W44" s="59">
+        <f>SUM($M$21:$M$24)*(1/(1/6+SUM('S2_1946-1970'!$H$6:$H$7)))</f>
+        <v>263.14444444444445</v>
+      </c>
+      <c r="X44" s="230" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="45" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A45" s="127"/>
       <c r="B45" s="104"/>
+      <c r="Q45" s="233" t="s">
+        <v>172</v>
+      </c>
+      <c r="R45" s="231" t="s">
+        <v>118</v>
+      </c>
+      <c r="S45" s="59">
+        <f>$M$30*(1/(1/3+SUM(S1_EPB2010!$H$26:$H$27)))</f>
+        <v>159.28723404255319</v>
+      </c>
+      <c r="T45" s="230" t="s">
+        <v>119</v>
+      </c>
+      <c r="U45" s="233" t="s">
+        <v>172</v>
+      </c>
+      <c r="V45" s="231" t="s">
+        <v>118</v>
+      </c>
+      <c r="W45" s="59">
+        <f>$M30*(1/(1/3+SUM('S2_1946-1970'!$H$37:$H$38)))</f>
+        <v>147.21862348178138</v>
+      </c>
+      <c r="X45" s="230" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="46" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Q46" s="233" t="s">
+        <v>173</v>
+      </c>
+      <c r="R46" s="231" t="s">
+        <v>118</v>
+      </c>
+      <c r="S46" s="59">
+        <f>$M$32*1/(2*SUM(S1_EPB2010!$H$33:$H$35)/4+1/8)</f>
+        <v>287.79925650557618</v>
+      </c>
+      <c r="T46" s="230" t="s">
+        <v>119</v>
+      </c>
+      <c r="U46" s="233" t="s">
+        <v>173</v>
+      </c>
+      <c r="V46" s="231" t="s">
+        <v>118</v>
+      </c>
+      <c r="W46" s="59">
+        <f>$M$32*1/(2*SUM('S2_1946-1970'!$H$29:$H$31)/4+1/8)</f>
+        <v>264.22525597269623</v>
+      </c>
+      <c r="X46" s="230" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="47" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Q47" s="233" t="s">
+        <v>174</v>
+      </c>
+      <c r="R47" s="231" t="s">
+        <v>118</v>
+      </c>
+      <c r="S47" s="59">
+        <f>$M$20*2/20*1.204*1012/3600+2*SUM($M$29)*S1_EPB2010!$H$44+S1_EPB2010!$H$54*SUM($S$2:$S$5)</f>
+        <v>48.734869629173538</v>
+      </c>
+      <c r="T47" s="230" t="s">
+        <v>119</v>
+      </c>
+      <c r="U47" s="233" t="s">
+        <v>174</v>
+      </c>
+      <c r="V47" s="231" t="s">
+        <v>118</v>
+      </c>
+      <c r="W47" s="59">
+        <f>$M$20*10/20*1.204*1012/3600+(2*$M$29)*(1/(1/8+'S2_1946-1970'!H40))+'S2_1946-1970'!H50*SUM($S$2:$S$5)</f>
+        <v>71.046484380114038</v>
+      </c>
+      <c r="X47" s="230" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="48" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Q48" s="233" t="s">
+        <v>175</v>
+      </c>
+      <c r="R48" s="231" t="s">
+        <v>118</v>
+      </c>
+      <c r="S48" s="230">
+        <f>SUM($M$21:$M$24)*(1/(1/23+SUM(S1_EPB2010!$H$4:$H$6)))</f>
+        <v>43.471808036604997</v>
+      </c>
+      <c r="T48" s="230" t="s">
+        <v>119</v>
+      </c>
+      <c r="U48" s="233" t="s">
+        <v>175</v>
+      </c>
+      <c r="V48" s="231" t="s">
+        <v>118</v>
+      </c>
+      <c r="W48" s="230">
+        <f>SUM($M21:$M24)*(1/(1/23+SUM('S2_1946-1970'!$H$4:$H$5)))</f>
+        <v>290.74406191619971</v>
+      </c>
+      <c r="X48" s="230" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="49" spans="17:24" x14ac:dyDescent="0.25">
+      <c r="Q49" s="233" t="s">
+        <v>176</v>
+      </c>
+      <c r="R49" s="231" t="s">
+        <v>118</v>
+      </c>
+      <c r="S49" s="59">
+        <f>$M$30*1/(SUM(S1_EPB2010!$H$28:$H$29))/2</f>
+        <v>16.197327394209353</v>
+      </c>
+      <c r="T49" s="230" t="s">
+        <v>119</v>
+      </c>
+      <c r="U49" s="233" t="s">
+        <v>176</v>
+      </c>
+      <c r="V49" s="231" t="s">
+        <v>118</v>
+      </c>
+      <c r="W49" s="59">
+        <f>$M30*1/(SUM('S2_1946-1970'!$H$25))/2</f>
+        <v>505.04166666666663</v>
+      </c>
+      <c r="X49" s="230" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="50" spans="17:24" x14ac:dyDescent="0.25">
+      <c r="Q50"/>
+      <c r="R50" s="231"/>
+      <c r="T50" s="230"/>
+      <c r="U50"/>
+      <c r="V50" s="231"/>
+      <c r="X50" s="230"/>
+    </row>
+    <row r="51" spans="17:24" x14ac:dyDescent="0.25">
+      <c r="Q51" s="178" t="s">
+        <v>214</v>
+      </c>
+      <c r="R51" s="230" t="s">
+        <v>118</v>
+      </c>
+      <c r="S51" s="59">
+        <f>S8*S1_EPB2010!$C$55*0.33*0.8</f>
+        <v>0.57802799999999999</v>
+      </c>
+      <c r="T51" s="230" t="s">
+        <v>119</v>
+      </c>
+      <c r="U51" s="178" t="s">
+        <v>214</v>
+      </c>
+      <c r="V51" s="230" t="s">
+        <v>118</v>
+      </c>
+      <c r="W51" s="59">
+        <f>W8*'S2_1946-1970'!$C$51*0.33*0.8</f>
+        <v>0.57802799999999999</v>
+      </c>
+      <c r="X51" s="230" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="52" spans="17:24" x14ac:dyDescent="0.25">
+      <c r="Q52" s="178" t="s">
+        <v>215</v>
+      </c>
+      <c r="R52" s="230" t="s">
+        <v>118</v>
+      </c>
+      <c r="S52" s="59">
+        <f>S2*S1_EPB2010!$C$55*0.33*0.8</f>
+        <v>0.35877600000000004</v>
+      </c>
+      <c r="T52" s="230" t="s">
+        <v>119</v>
+      </c>
+      <c r="U52" s="178" t="s">
+        <v>215</v>
+      </c>
+      <c r="V52" s="230" t="s">
+        <v>118</v>
+      </c>
+      <c r="W52" s="59">
+        <f>W2*'S2_1946-1970'!$C$51*0.33*0.8</f>
+        <v>0.35877600000000004</v>
+      </c>
+      <c r="X52" s="230" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="53" spans="17:24" x14ac:dyDescent="0.25">
+      <c r="Q53" s="178" t="s">
+        <v>216</v>
+      </c>
+      <c r="R53" s="230" t="s">
+        <v>118</v>
+      </c>
+      <c r="S53" s="59">
+        <f>S4*S1_EPB2010!$C$55*0.33*0.8</f>
+        <v>1.4032128000000001</v>
+      </c>
+      <c r="T53" s="230" t="s">
+        <v>119</v>
+      </c>
+      <c r="U53" s="178" t="s">
+        <v>216</v>
+      </c>
+      <c r="V53" s="230" t="s">
+        <v>118</v>
+      </c>
+      <c r="W53" s="59">
+        <f>W4*'S2_1946-1970'!$C$51*0.33*0.8</f>
+        <v>1.4032128000000001</v>
+      </c>
+      <c r="X53" s="230" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="54" spans="17:24" x14ac:dyDescent="0.25">
+      <c r="Q54" s="178" t="s">
+        <v>217</v>
+      </c>
+      <c r="R54" s="230" t="s">
+        <v>118</v>
+      </c>
+      <c r="S54" s="59">
+        <f>S5*S1_EPB2010!$C$55*0.33*0.8</f>
+        <v>1.1241648</v>
+      </c>
+      <c r="T54" s="230" t="s">
+        <v>119</v>
+      </c>
+      <c r="U54" s="178" t="s">
+        <v>217</v>
+      </c>
+      <c r="V54" s="230" t="s">
+        <v>118</v>
+      </c>
+      <c r="W54" s="59">
+        <f>W5*'S2_1946-1970'!$C$51*0.33*0.8</f>
+        <v>1.1241648</v>
+      </c>
+      <c r="X54" s="230" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="55" spans="17:24" x14ac:dyDescent="0.25">
+      <c r="Q55" s="178" t="s">
+        <v>218</v>
+      </c>
+      <c r="R55" s="230" t="s">
+        <v>118</v>
+      </c>
+      <c r="S55" s="59">
+        <f>S51</f>
+        <v>0.57802799999999999</v>
+      </c>
+      <c r="T55" s="230" t="s">
+        <v>119</v>
+      </c>
+      <c r="U55" s="178" t="s">
+        <v>218</v>
+      </c>
+      <c r="V55" s="230" t="s">
+        <v>118</v>
+      </c>
+      <c r="W55" s="59">
+        <f>W51</f>
+        <v>0.57802799999999999</v>
+      </c>
+      <c r="X55" s="230" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="56" spans="17:24" x14ac:dyDescent="0.25">
+      <c r="Q56" s="178" t="s">
+        <v>219</v>
+      </c>
+      <c r="R56" s="230" t="s">
+        <v>118</v>
+      </c>
+      <c r="S56" s="59">
+        <f t="shared" ref="S56:S58" si="5">S52</f>
+        <v>0.35877600000000004</v>
+      </c>
+      <c r="T56" s="230" t="s">
+        <v>119</v>
+      </c>
+      <c r="U56" s="178" t="s">
+        <v>219</v>
+      </c>
+      <c r="V56" s="230" t="s">
+        <v>118</v>
+      </c>
+      <c r="W56" s="59">
+        <f t="shared" ref="W56:W58" si="6">W52</f>
+        <v>0.35877600000000004</v>
+      </c>
+      <c r="X56" s="230" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="57" spans="17:24" x14ac:dyDescent="0.25">
+      <c r="Q57" s="178" t="s">
+        <v>220</v>
+      </c>
+      <c r="R57" s="230" t="s">
+        <v>118</v>
+      </c>
+      <c r="S57" s="59">
+        <f t="shared" si="5"/>
+        <v>1.4032128000000001</v>
+      </c>
+      <c r="T57" s="230" t="s">
+        <v>119</v>
+      </c>
+      <c r="U57" s="178" t="s">
+        <v>220</v>
+      </c>
+      <c r="V57" s="230" t="s">
+        <v>118</v>
+      </c>
+      <c r="W57" s="59">
+        <f t="shared" si="6"/>
+        <v>1.4032128000000001</v>
+      </c>
+      <c r="X57" s="230" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="58" spans="17:24" x14ac:dyDescent="0.25">
+      <c r="Q58" s="178" t="s">
+        <v>221</v>
+      </c>
+      <c r="R58" s="230" t="s">
+        <v>118</v>
+      </c>
+      <c r="S58" s="59">
+        <f t="shared" si="5"/>
+        <v>1.1241648</v>
+      </c>
+      <c r="T58" s="230" t="s">
+        <v>119</v>
+      </c>
+      <c r="U58" s="178" t="s">
+        <v>221</v>
+      </c>
+      <c r="V58" s="230" t="s">
+        <v>118</v>
+      </c>
+      <c r="W58" s="59">
+        <f t="shared" si="6"/>
+        <v>1.1241648</v>
+      </c>
+      <c r="X58" s="230" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="59" spans="17:24" x14ac:dyDescent="0.25">
+      <c r="Q59" s="178" t="s">
+        <v>222</v>
+      </c>
+      <c r="R59" s="230" t="s">
+        <v>118</v>
+      </c>
+      <c r="S59" s="59">
+        <v>0</v>
+      </c>
+      <c r="T59" s="230" t="s">
+        <v>119</v>
+      </c>
+      <c r="U59" s="178" t="s">
+        <v>222</v>
+      </c>
+      <c r="V59" s="230" t="s">
+        <v>118</v>
+      </c>
+      <c r="W59" s="59">
+        <v>0</v>
+      </c>
+      <c r="X59" s="230" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="60" spans="17:24" x14ac:dyDescent="0.25">
+      <c r="Q60" s="178" t="s">
+        <v>223</v>
+      </c>
+      <c r="R60" s="230" t="s">
+        <v>118</v>
+      </c>
+      <c r="S60" s="59">
+        <v>0</v>
+      </c>
+      <c r="T60" s="230" t="s">
+        <v>119</v>
+      </c>
+      <c r="U60" s="178" t="s">
+        <v>223</v>
+      </c>
+      <c r="V60" s="230" t="s">
+        <v>118</v>
+      </c>
+      <c r="W60" s="59">
+        <v>0</v>
+      </c>
+      <c r="X60" s="230" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="61" spans="17:24" x14ac:dyDescent="0.25">
+      <c r="Q61" s="178" t="s">
+        <v>224</v>
+      </c>
+      <c r="R61" s="230" t="s">
+        <v>118</v>
+      </c>
+      <c r="S61" s="59">
+        <v>0</v>
+      </c>
+      <c r="T61" s="230" t="s">
+        <v>119</v>
+      </c>
+      <c r="U61" s="178" t="s">
+        <v>224</v>
+      </c>
+      <c r="V61" s="230" t="s">
+        <v>118</v>
+      </c>
+      <c r="W61" s="59">
+        <v>0</v>
+      </c>
+      <c r="X61" s="230" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="62" spans="17:24" x14ac:dyDescent="0.25">
+      <c r="Q62" s="178" t="s">
+        <v>225</v>
+      </c>
+      <c r="R62" s="230" t="s">
+        <v>118</v>
+      </c>
+      <c r="S62" s="59">
+        <v>0</v>
+      </c>
+      <c r="T62" s="230" t="s">
+        <v>119</v>
+      </c>
+      <c r="U62" s="178" t="s">
+        <v>225</v>
+      </c>
+      <c r="V62" s="230" t="s">
+        <v>118</v>
+      </c>
+      <c r="W62" s="59">
+        <v>0</v>
+      </c>
+      <c r="X62" s="230" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="63" spans="17:24" x14ac:dyDescent="0.25">
+      <c r="Q63" s="178" t="s">
+        <v>226</v>
+      </c>
+      <c r="R63" s="230" t="s">
+        <v>118</v>
+      </c>
+      <c r="S63" s="59">
+        <f>S55</f>
+        <v>0.57802799999999999</v>
+      </c>
+      <c r="T63" s="230" t="s">
+        <v>119</v>
+      </c>
+      <c r="U63" s="178" t="s">
+        <v>226</v>
+      </c>
+      <c r="V63" s="230" t="s">
+        <v>118</v>
+      </c>
+      <c r="W63" s="59">
+        <f>W55</f>
+        <v>0.57802799999999999</v>
+      </c>
+      <c r="X63" s="230" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="64" spans="17:24" x14ac:dyDescent="0.25">
+      <c r="Q64" s="178" t="s">
+        <v>227</v>
+      </c>
+      <c r="R64" s="230" t="s">
+        <v>118</v>
+      </c>
+      <c r="S64" s="59">
+        <f>S56</f>
+        <v>0.35877600000000004</v>
+      </c>
+      <c r="T64" s="230" t="s">
+        <v>119</v>
+      </c>
+      <c r="U64" s="178" t="s">
+        <v>227</v>
+      </c>
+      <c r="V64" s="230" t="s">
+        <v>118</v>
+      </c>
+      <c r="W64" s="59">
+        <f>W56</f>
+        <v>0.35877600000000004</v>
+      </c>
+      <c r="X64" s="230" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="65" spans="17:24" x14ac:dyDescent="0.25">
+      <c r="Q65" s="178" t="s">
+        <v>228</v>
+      </c>
+      <c r="R65" s="230" t="s">
+        <v>118</v>
+      </c>
+      <c r="S65" s="59">
+        <f>S57</f>
+        <v>1.4032128000000001</v>
+      </c>
+      <c r="T65" s="230" t="s">
+        <v>119</v>
+      </c>
+      <c r="U65" s="178" t="s">
+        <v>228</v>
+      </c>
+      <c r="V65" s="230" t="s">
+        <v>118</v>
+      </c>
+      <c r="W65" s="59">
+        <f>W57</f>
+        <v>1.4032128000000001</v>
+      </c>
+      <c r="X65" s="230" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="66" spans="17:24" x14ac:dyDescent="0.25">
+      <c r="Q66" s="178" t="s">
+        <v>229</v>
+      </c>
+      <c r="R66" s="230" t="s">
+        <v>118</v>
+      </c>
+      <c r="S66" s="59">
+        <f>S58</f>
+        <v>1.1241648</v>
+      </c>
+      <c r="T66" s="230" t="s">
+        <v>119</v>
+      </c>
+      <c r="U66" s="178" t="s">
+        <v>229</v>
+      </c>
+      <c r="V66" s="230" t="s">
+        <v>118</v>
+      </c>
+      <c r="W66" s="59">
+        <f>W58</f>
+        <v>1.1241648</v>
+      </c>
+      <c r="X66" s="230" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="67" spans="17:24" x14ac:dyDescent="0.25">
+      <c r="Q67"/>
+      <c r="R67" s="231"/>
+      <c r="T67" s="230"/>
+      <c r="U67"/>
+      <c r="V67" s="231"/>
+      <c r="X67" s="230"/>
+    </row>
+    <row r="68" spans="17:24" x14ac:dyDescent="0.25">
+      <c r="Q68" s="233" t="s">
+        <v>177</v>
+      </c>
+      <c r="R68" s="231" t="s">
+        <v>118</v>
+      </c>
+      <c r="S68" s="236">
+        <f>($M$7+$M$2)*1.204*1012*5</f>
+        <v>1779786.9935999999</v>
+      </c>
+      <c r="T68" s="230" t="s">
+        <v>119</v>
+      </c>
+      <c r="U68" s="233" t="s">
+        <v>177</v>
+      </c>
+      <c r="V68" s="231" t="s">
+        <v>118</v>
+      </c>
+      <c r="W68" s="236">
+        <f>($M7+$M2)*1.204*1012*5</f>
+        <v>1779786.9935999999</v>
+      </c>
+      <c r="X68" s="230" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="69" spans="17:24" x14ac:dyDescent="0.25">
+      <c r="Q69" s="233" t="s">
+        <v>178</v>
+      </c>
+      <c r="R69" s="231" t="s">
+        <v>118</v>
+      </c>
+      <c r="S69" s="236">
+        <f>SUM($M$5:$M$6,$M$8:$M$11)*SUM(S1_EPB2010!$I$7:$I$8)+SUM($M$3:$M$4,$M$16:$M$17)*SUM(S1_EPB2010!$I$15:$I$16)</f>
+        <v>17636327.200000003</v>
+      </c>
+      <c r="T69" s="230" t="s">
+        <v>119</v>
+      </c>
+      <c r="U69" s="233" t="s">
+        <v>178</v>
+      </c>
+      <c r="V69" s="231" t="s">
+        <v>118</v>
+      </c>
+      <c r="W69" s="236">
+        <f>SUM($M$5:M6,$M$8:M11)*SUM('S2_1946-1970'!$I$6:$I$7)+SUM($M$3:M4,$M$16:$M17)*SUM('S2_1946-1970'!$I$13)</f>
+        <v>29091367.200000003</v>
+      </c>
+      <c r="X69" s="230" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="70" spans="17:24" x14ac:dyDescent="0.25">
+      <c r="Q70" s="233" t="s">
+        <v>179</v>
+      </c>
+      <c r="R70" s="231" t="s">
+        <v>118</v>
+      </c>
+      <c r="S70" s="236">
+        <f>SUM($M$18)*SUM(S1_EPB2010!$I$33:$I$35)+SUM($M$19)*SUM(S1_EPB2010!$I$39:$I$42)</f>
+        <v>47109546</v>
+      </c>
+      <c r="T70" s="230" t="s">
+        <v>119</v>
+      </c>
+      <c r="U70" s="233" t="s">
+        <v>179</v>
+      </c>
+      <c r="V70" s="231" t="s">
+        <v>118</v>
+      </c>
+      <c r="W70" s="236">
+        <f>SUM($M18)*SUM('S2_1946-1970'!$I$29:$I$31)+(M19)*SUM('S2_1946-1970'!$I$35:$I$38)</f>
+        <v>51331734</v>
+      </c>
+      <c r="X70" s="230" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="71" spans="17:24" x14ac:dyDescent="0.25">
+      <c r="Q71" s="233" t="s">
+        <v>180</v>
+      </c>
+      <c r="R71" s="231" t="s">
+        <v>118</v>
+      </c>
+      <c r="S71" s="59">
+        <v>0.1</v>
+      </c>
+      <c r="T71" s="230" t="s">
+        <v>119</v>
+      </c>
+      <c r="U71" s="233" t="s">
+        <v>180</v>
+      </c>
+      <c r="V71" s="231" t="s">
+        <v>118</v>
+      </c>
+      <c r="W71" s="59">
+        <v>0.1</v>
+      </c>
+      <c r="X71" s="230" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="72" spans="17:24" x14ac:dyDescent="0.25">
+      <c r="Q72" s="233" t="s">
+        <v>181</v>
+      </c>
+      <c r="R72" s="231" t="s">
+        <v>118</v>
+      </c>
+      <c r="S72" s="59">
+        <v>0.1</v>
+      </c>
+      <c r="T72" s="230" t="s">
+        <v>119</v>
+      </c>
+      <c r="U72" s="233" t="s">
+        <v>181</v>
+      </c>
+      <c r="V72" s="231" t="s">
+        <v>118</v>
+      </c>
+      <c r="W72" s="59">
+        <v>0.1</v>
+      </c>
+      <c r="X72" s="230" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="73" spans="17:24" x14ac:dyDescent="0.25">
+      <c r="Q73" s="233" t="s">
+        <v>182</v>
+      </c>
+      <c r="R73" s="231" t="s">
+        <v>118</v>
+      </c>
+      <c r="S73" s="59">
+        <v>0.7</v>
+      </c>
+      <c r="T73" s="230" t="s">
+        <v>119</v>
+      </c>
+      <c r="U73" s="233" t="s">
+        <v>182</v>
+      </c>
+      <c r="V73" s="231" t="s">
+        <v>118</v>
+      </c>
+      <c r="W73" s="59">
+        <v>0.7</v>
+      </c>
+      <c r="X73" s="230" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="74" spans="17:24" x14ac:dyDescent="0.25">
+      <c r="Q74"/>
+      <c r="R74" s="231"/>
+      <c r="T74" s="230"/>
+      <c r="U74"/>
+      <c r="V74" s="231"/>
+      <c r="X74" s="230"/>
+    </row>
+    <row r="75" spans="17:24" x14ac:dyDescent="0.25">
+      <c r="Q75" s="233" t="s">
+        <v>183</v>
+      </c>
+      <c r="R75" s="231" t="s">
+        <v>118</v>
+      </c>
+      <c r="S75" s="59">
+        <f>SUM($M$8:$M$11)*1/(1/6+SUM(S1_EPB2010!$H$7:$H$8))+SUM($M$3:$M$4,$M$16:$M$17)*1/(1/10+SUM(S1_EPB2010!$H$15:$H$16))</f>
+        <v>540.02598752598749</v>
+      </c>
+      <c r="T75" s="230" t="s">
+        <v>119</v>
+      </c>
+      <c r="U75" s="233" t="s">
+        <v>183</v>
+      </c>
+      <c r="V75" s="231" t="s">
+        <v>118</v>
+      </c>
+      <c r="W75" s="59">
+        <f>SUM($M$8:M11,M5:M6)*1/(1/6+SUM('S2_1946-1970'!$I$6:$I$7))+SUM($M$3:$M4,M16:M17)*1/(1/10+SUM('S2_1946-1970'!$H$13))</f>
+        <v>822.00049876001071</v>
+      </c>
+      <c r="X75" s="230" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="76" spans="17:24" x14ac:dyDescent="0.25">
+      <c r="Q76" s="233" t="s">
+        <v>184</v>
+      </c>
+      <c r="R76" s="231" t="s">
+        <v>118</v>
+      </c>
+      <c r="S76" s="59">
+        <f>$M$18*1/(1/8+SUM(S1_EPB2010!$H$33:$H$35)/4)+SUM($M$19)*1/(1/3+SUM(S1_EPB2010!$H$39:$H$42)/2)</f>
+        <v>496.70196507003857</v>
+      </c>
+      <c r="T76" s="230" t="s">
+        <v>119</v>
+      </c>
+      <c r="U76" s="233" t="s">
+        <v>184</v>
+      </c>
+      <c r="V76" s="231" t="s">
+        <v>118</v>
+      </c>
+      <c r="W76" s="59">
+        <f>M18*1/(1/8+SUM('S2_1946-1970'!$H$29:$H$31)/4)+SUM($M$19)*1/(1/3+SUM('S2_1946-1970'!$H$35:$H$38)/2)</f>
+        <v>459.94024051058108</v>
+      </c>
+      <c r="X76" s="230" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="77" spans="17:24" x14ac:dyDescent="0.25">
+      <c r="Q77" s="233" t="s">
+        <v>185</v>
+      </c>
+      <c r="R77" s="231" t="s">
+        <v>118</v>
+      </c>
+      <c r="S77" s="59">
+        <f>($M$2+$M$7)*2/20*1.204*1012/3600+SUM($S$7:$S$10)*S1_EPB2010!$H$54</f>
+        <v>26.633205519999997</v>
+      </c>
+      <c r="T77" s="230" t="s">
+        <v>119</v>
+      </c>
+      <c r="U77" s="233" t="s">
+        <v>185</v>
+      </c>
+      <c r="V77" s="231" t="s">
+        <v>118</v>
+      </c>
+      <c r="W77" s="59">
+        <f>($M$2+$M$7)*10/20*1.204*1012/3600+SUM($S$7:$S$10)*'S2_1946-1970'!$H$50</f>
+        <v>66.184027600000007</v>
+      </c>
+      <c r="X77" s="230" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="78" spans="17:24" x14ac:dyDescent="0.25">
+      <c r="Q78" s="233" t="s">
+        <v>186</v>
+      </c>
+      <c r="R78" s="231" t="s">
+        <v>118</v>
+      </c>
+      <c r="S78" s="230">
+        <f>SUM($M$8:$M$11)*1/(1/23+SUM(S1_EPB2010!$H$4:$H$6))+SUM($M$3:$M$4,$M$16:$M$17)*1/(1/23+SUM(S1_EPB2010!$H$12:$H$14))</f>
+        <v>89.005091905312511</v>
+      </c>
+      <c r="T78" s="230" t="s">
+        <v>119</v>
+      </c>
+      <c r="U78" s="233" t="s">
+        <v>186</v>
+      </c>
+      <c r="V78" s="231" t="s">
+        <v>118</v>
+      </c>
+      <c r="W78" s="230">
+        <f>SUM($M$8:$M$11,M5:M6)*1/(1/23+SUM('S2_1946-1970'!$H$4:$H$5))+SUM($M$3:M4,M$16:M17)*1/(1/23+SUM('S2_1946-1970'!$H$11:$H$12))</f>
+        <v>894.68583701517059</v>
+      </c>
+      <c r="X78" s="230" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="79" spans="17:24" x14ac:dyDescent="0.25">
+      <c r="Q79"/>
+      <c r="R79" s="231"/>
+      <c r="T79" s="230"/>
+      <c r="U79"/>
+      <c r="V79" s="231"/>
+      <c r="X79" s="230"/>
+    </row>
+    <row r="80" spans="17:24" x14ac:dyDescent="0.25">
+      <c r="Q80" s="233" t="s">
+        <v>187</v>
+      </c>
+      <c r="R80" s="231" t="s">
+        <v>118</v>
+      </c>
+      <c r="S80" s="59">
+        <f>$M$33*SUM(S1_EPB2010!$I$39:$I$42)/2</f>
+        <v>18239253</v>
+      </c>
+      <c r="T80" s="230" t="s">
+        <v>119</v>
+      </c>
+      <c r="U80" s="233" t="s">
+        <v>187</v>
+      </c>
+      <c r="V80" s="231" t="s">
+        <v>118</v>
+      </c>
+      <c r="W80" s="59">
+        <f>$M$33*SUM('S2_1946-1970'!$I$35:$I$38)/2</f>
+        <v>18594327</v>
+      </c>
+      <c r="X80" s="230" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="81" spans="17:24" x14ac:dyDescent="0.25">
+      <c r="Q81" s="233" t="s">
+        <v>188</v>
+      </c>
+      <c r="R81" s="231" t="s">
+        <v>118</v>
+      </c>
+      <c r="S81" s="59">
+        <f>$S$80</f>
+        <v>18239253</v>
+      </c>
+      <c r="T81" s="230" t="s">
+        <v>119</v>
+      </c>
+      <c r="U81" s="233" t="s">
+        <v>188</v>
+      </c>
+      <c r="V81" s="231" t="s">
+        <v>118</v>
+      </c>
+      <c r="W81" s="59">
+        <f>W80</f>
+        <v>18594327</v>
+      </c>
+      <c r="X81" s="230" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="82" spans="17:24" x14ac:dyDescent="0.25">
+      <c r="Q82" s="233" t="s">
+        <v>189</v>
+      </c>
+      <c r="R82" s="231" t="s">
+        <v>118</v>
+      </c>
+      <c r="S82" s="59">
+        <v>0.1</v>
+      </c>
+      <c r="T82" s="230" t="s">
+        <v>119</v>
+      </c>
+      <c r="U82" s="233" t="s">
+        <v>189</v>
+      </c>
+      <c r="V82" s="231" t="s">
+        <v>118</v>
+      </c>
+      <c r="W82" s="59">
+        <v>0.1</v>
+      </c>
+      <c r="X82" s="230" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="83" spans="17:24" x14ac:dyDescent="0.25">
+      <c r="Q83" s="233" t="s">
+        <v>190</v>
+      </c>
+      <c r="R83" s="231" t="s">
+        <v>118</v>
+      </c>
+      <c r="S83" s="59">
+        <v>0.1</v>
+      </c>
+      <c r="T83" s="230" t="s">
+        <v>119</v>
+      </c>
+      <c r="U83" s="233" t="s">
+        <v>190</v>
+      </c>
+      <c r="V83" s="231" t="s">
+        <v>118</v>
+      </c>
+      <c r="W83" s="59">
+        <v>0.1</v>
+      </c>
+      <c r="X83" s="230" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="84" spans="17:24" x14ac:dyDescent="0.25">
+      <c r="Q84" s="233" t="s">
+        <v>191</v>
+      </c>
+      <c r="R84" s="231" t="s">
+        <v>118</v>
+      </c>
+      <c r="S84" s="59">
+        <f>1/S1_EPB2010!$H$37*4*$M$33</f>
+        <v>151.70722689075629</v>
+      </c>
+      <c r="T84" s="230" t="s">
+        <v>119</v>
+      </c>
+      <c r="U84" s="233" t="s">
+        <v>191</v>
+      </c>
+      <c r="V84" s="231" t="s">
+        <v>118</v>
+      </c>
+      <c r="W84" s="59">
+        <f>1/'S2_1946-1970'!$H$33*4*$M$33</f>
+        <v>188.82849673202614</v>
+      </c>
+      <c r="X84" s="230" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="85" spans="17:24" x14ac:dyDescent="0.25">
+      <c r="Q85" s="233" t="s">
+        <v>192</v>
+      </c>
+      <c r="R85" s="231" t="s">
+        <v>118</v>
+      </c>
+      <c r="S85" s="59">
+        <f>$S$84*2</f>
+        <v>303.41445378151258</v>
+      </c>
+      <c r="T85" s="230" t="s">
+        <v>119</v>
+      </c>
+      <c r="U85" s="233" t="s">
+        <v>192</v>
+      </c>
+      <c r="V85" s="231" t="s">
+        <v>118</v>
+      </c>
+      <c r="W85" s="59">
+        <f>$S$84*2</f>
+        <v>303.41445378151258</v>
+      </c>
+      <c r="X85" s="230" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="86" spans="17:24" x14ac:dyDescent="0.25">
+      <c r="Q86" s="233" t="s">
+        <v>193</v>
+      </c>
+      <c r="R86" s="231" t="s">
+        <v>118</v>
+      </c>
+      <c r="S86" s="59">
+        <f>$S$84</f>
+        <v>151.70722689075629</v>
+      </c>
+      <c r="T86" s="230" t="s">
+        <v>119</v>
+      </c>
+      <c r="U86" s="233" t="s">
+        <v>193</v>
+      </c>
+      <c r="V86" s="231" t="s">
+        <v>118</v>
+      </c>
+      <c r="W86" s="59">
+        <f>$S$84</f>
+        <v>151.70722689075629</v>
+      </c>
+      <c r="X86" s="230" t="s">
+        <v>119</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="3">
     <mergeCell ref="I36:N38"/>
+    <mergeCell ref="Q1:T1"/>
+    <mergeCell ref="U1:X1"/>
   </mergeCells>
   <conditionalFormatting sqref="D32:D39">
     <cfRule type="iconSet" priority="2">
@@ -6325,8 +8386,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AF86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="X1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView topLeftCell="T28" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="AE38" sqref="AE38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6682,7 +8743,7 @@
         <v>118</v>
       </c>
       <c r="AE4" s="234">
-        <f t="shared" ref="AE4:AE10" si="1">W4</f>
+        <f t="shared" ref="AE4:AE5" si="1">W4</f>
         <v>2.8600000000000003</v>
       </c>
       <c r="AF4" s="230" t="s">
@@ -6900,7 +8961,7 @@
         <v>118</v>
       </c>
       <c r="AE7" s="234">
-        <f t="shared" ref="AE7:AE13" si="2">W7</f>
+        <f t="shared" ref="AE7:AE10" si="2">W7</f>
         <v>1.6</v>
       </c>
       <c r="AF7" s="230" t="s">
@@ -9276,8 +11337,8 @@
         <v>118</v>
       </c>
       <c r="AA37" s="235">
-        <f>SUM($L$28)*SUM('S2_1946-1970'!$I$37:$I$38)</f>
-        <v>37153809.000000007</v>
+        <f>SUM($L$28)*SUM('S2_1946-1970'!$I$23:$I$24)</f>
+        <v>7312459.0000000009</v>
       </c>
       <c r="AB37" s="230" t="s">
         <v>119</v>
@@ -9289,8 +11350,8 @@
         <v>118</v>
       </c>
       <c r="AE37" s="235">
-        <f>SUM($L$28)*SUM('S2_1946-1970'!$I$37:$I$38)</f>
-        <v>37153809.000000007</v>
+        <f>SUM($L$28)*SUM('S2_1946-1970'!$I$23:$I$24)</f>
+        <v>7312459.0000000009</v>
       </c>
       <c r="AF37" s="230" t="s">
         <v>119</v>
@@ -11754,8 +13815,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X86"/>
   <sheetViews>
-    <sheetView topLeftCell="S53" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="U2" sqref="U2:X86"/>
+    <sheetView topLeftCell="H1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="W37" sqref="W37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13802,8 +15863,8 @@
         <v>118</v>
       </c>
       <c r="W37" s="235">
-        <f>SUM($L$26)*SUM('S2_1946-1970'!$I$37:$I$38)</f>
-        <v>24484590.900000002</v>
+        <f>SUM($L$26)*SUM('S2_1946-1970'!$I$23:$I$24)</f>
+        <v>4818955.9000000004</v>
       </c>
       <c r="X37" s="230" t="s">
         <v>119</v>
@@ -14135,8 +16196,8 @@
         <v>118</v>
       </c>
       <c r="W47" s="59">
-        <f>$L$17*2/20*1.204*1012/3600+($L$24+$L$25)*(1/(1/8+'S2_1946-1970'!H40))+'S2_1946-1970'!H50*SUM($S$2:$S$5)</f>
-        <v>19.366630830435959</v>
+        <f>$L$17*10/20*1.204*1012/3600+($L$24+$L$25)*(1/(1/8+'S2_1946-1970'!H40))+'S2_1946-1970'!H50*SUM($S$2:$S$5)</f>
+        <v>38.121083983769289</v>
       </c>
       <c r="X47" s="230" t="s">
         <v>119</v>
@@ -14697,8 +16758,8 @@
         <v>118</v>
       </c>
       <c r="S69" s="236">
-        <f>SUM($L$7,$L$9)*SUM(S1_EPB2010!$I$7:$I$8)+SUM($L$3)*SUM(S1_EPB2010!$I$15:$I$16)</f>
-        <v>5989288.3088610489</v>
+        <f>SUM($L$7,$L$9)*SUM(S1_EPB2010!$I$7:$I$8)+SUM($L$3+$L$13)*SUM(S1_EPB2010!$I$15:$I$16)</f>
+        <v>6377285.7405068344</v>
       </c>
       <c r="T69" s="230" t="s">
         <v>119</v>
@@ -14710,8 +16771,8 @@
         <v>118</v>
       </c>
       <c r="W69" s="236">
-        <f>SUM($L$9,$L$7)*SUM('S2_1946-1970'!$I$6:$I$7)+SUM($L$3)*SUM('S2_1946-1970'!$I$12:$I$13)</f>
-        <v>10999266.960905127</v>
+        <f>SUM($L$9,$L$7)*SUM('S2_1946-1970'!$I$6:$I$7)+SUM($L$3+$L$13)*SUM('S2_1946-1970'!$I$13)</f>
+        <v>11170756.38158397</v>
       </c>
       <c r="X69" s="230" t="s">
         <v>119</v>
@@ -14839,8 +16900,8 @@
         <v>118</v>
       </c>
       <c r="S75" s="59">
-        <f>SUM($L$7,$L$9)*1/(1/6+SUM(S1_EPB2010!$H$7:$H$8))+SUM($L$3)*1/(1/10+SUM(S1_EPB2010!$H$15:$H$16))</f>
-        <v>141.49780233506308</v>
+        <f>SUM($L$7,$L$9)*1/(1/6+SUM(S1_EPB2010!$H$7:$H$8))+SUM($L$3+$L$13)*1/(1/10+SUM(S1_EPB2010!$H$15:$H$16))</f>
+        <v>174.71813953334583</v>
       </c>
       <c r="T75" s="230" t="s">
         <v>119</v>
@@ -14852,8 +16913,8 @@
         <v>118</v>
       </c>
       <c r="W75" s="59">
-        <f>SUM($L$7,$L$9)*1/(1/6+SUM('S2_1946-1970'!$I$6:$I$7))+SUM($L$3)*1/(1/10+SUM('S2_1946-1970'!$H$11:$H$13))</f>
-        <v>58.173855015697661</v>
+        <f>SUM($L$7,$L$9)*1/(1/6+SUM('S2_1946-1970'!$I$6:$I$7))+SUM($L$3+L13)*1/(1/10+SUM('S2_1946-1970'!$H$13))</f>
+        <v>213.21538863852496</v>
       </c>
       <c r="X75" s="230" t="s">
         <v>119</v>
@@ -14908,8 +16969,8 @@
         <v>118</v>
       </c>
       <c r="W77" s="59">
-        <f>($L$2+$L$6)*2/20*1.204*1012/3600+SUM($S$7:$S$10)*'S2_1946-1970'!$H$50</f>
-        <v>30.685397641833333</v>
+        <f>($L$2+$L$6)*10/20*1.204*1012/3600+SUM($S$7:$S$10)*'S2_1946-1970'!$H$50</f>
+        <v>66.287788209166663</v>
       </c>
       <c r="X77" s="230" t="s">
         <v>119</v>
@@ -14923,8 +16984,8 @@
         <v>118</v>
       </c>
       <c r="S78" s="230">
-        <f>SUM($L$10,$L$12)*1/(1/23+SUM(S1_EPB2010!$H$4:$H$6))+SUM($L$3)*1/(1/23+SUM(S1_EPB2010!$H$12:$H$14))</f>
-        <v>32.816092241994802</v>
+        <f>SUM($L$10,$L$12)*1/(1/23+SUM(S1_EPB2010!$H$4:$H$6))+SUM($L$3+$L$13)*1/(1/23+SUM(S1_EPB2010!$H$12:$H$14))</f>
+        <v>36.298643118331256</v>
       </c>
       <c r="T78" s="230" t="s">
         <v>119</v>
@@ -14936,8 +16997,8 @@
         <v>118</v>
       </c>
       <c r="W78" s="230">
-        <f>SUM($L$10,$L$12)*1/(1/23+SUM('S2_1946-1970'!$H$4:$H$5))+SUM($L$3)*1/(1/23+SUM('S2_1946-1970'!$H$11:$H$12))</f>
-        <v>261.58012739529107</v>
+        <f>SUM($L$10,$L$12)*1/(1/23+SUM('S2_1946-1970'!$H$4:$H$5))+SUM($L$3+$L$13)*1/(1/23+SUM('S2_1946-1970'!$H$11:$H$12))</f>
+        <v>309.41573926819802</v>
       </c>
       <c r="X78" s="230" t="s">
         <v>119</v>

</xml_diff>